<commit_message>
Realize dos modificaciones - ocultes los input en crear pregunta - el documento que daniel pidio
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\git\mathusb2.0\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$D$9:$E$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$D$12:$E$31</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>Actividades</t>
   </si>
@@ -116,20 +116,29 @@
     <t>Realizado</t>
   </si>
   <si>
-    <t>Estudiante resuelve pregunta de documento</t>
-  </si>
-  <si>
-    <t>Modificar base de datos</t>
-  </si>
-  <si>
     <t>Ok</t>
+  </si>
+  <si>
+    <t>Estudiante puede responder pregunta abierta con unica respuesta en la plataforma</t>
+  </si>
+  <si>
+    <t>Estudiante puede responder pregunta de selecion multiple en la plataforma</t>
+  </si>
+  <si>
+    <t>Modificar base de datos para guardar resultados de las pruebas</t>
+  </si>
+  <si>
+    <t>Modificara base de datos para guardar preguntas con sus respectivas respuestas</t>
+  </si>
+  <si>
+    <t>Estudiante puede realizar examenes en la plataforma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +169,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -187,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -203,6 +218,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -296,6 +312,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -331,6 +364,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -483,22 +533,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F28"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="75.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="11.375" style="1"/>
+    <col min="5" max="5" width="78.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
@@ -506,245 +556,276 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="4">
+      <c r="F15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="4">
         <v>4</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="4">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="4">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="4">
-        <v>7</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="4">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" s="4">
+        <v>16</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="4">
+        <v>17</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="4">
+        <v>18</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="4">
         <v>19</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>31</v>
+      <c r="F31" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>